<commit_message>
player fire moved into playerclass
</commit_message>
<xml_diff>
--- a/Engine/data/datasheet/item_parameter.xlsx
+++ b/Engine/data/datasheet/item_parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC81BEF-D211-440D-8F6C-B87717697F2D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21841156-845C-45DF-A0C3-73F0F9996E88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="2190" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,10 +50,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SHOTGUN_FIRE_DELAY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>한번 쏠때 총알이 몇발씩</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -91,6 +87,10 @@
   </si>
   <si>
     <t>berserk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHOTGUN_BULLET_RELOAD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -535,7 +535,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:I32"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -549,10 +549,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -568,7 +568,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -610,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -624,12 +624,12 @@
         <v>0</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B7" s="9">
         <v>10</v>
@@ -638,23 +638,23 @@
         <v>1</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
shop item selectable and displayed
</commit_message>
<xml_diff>
--- a/Engine/data/datasheet/item_parameter.xlsx
+++ b/Engine/data/datasheet/item_parameter.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21841156-845C-45DF-A0C3-73F0F9996E88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB8745A-C1FB-4722-86D2-774C7852B26C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="2190" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32085" yWindow="1455" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>float</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,6 +91,14 @@
   </si>
   <si>
     <t>SHOTGUN_BULLET_RELOAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>siege</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>speedup</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -532,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -658,10 +666,23 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
+      <c r="A10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
+      <c r="A11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>